<commit_message>
Not sure what changes did here
</commit_message>
<xml_diff>
--- a/Run-time graph.xlsx
+++ b/Run-time graph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,12 +191,12 @@
         <c:gapWidth val="75"/>
         <c:gapDepth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="683921992"/>
-        <c:axId val="683857720"/>
+        <c:axId val="546434280"/>
+        <c:axId val="546427464"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="683921992"/>
+        <c:axId val="546434280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -232,7 +232,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="683857720"/>
+        <c:crossAx val="546427464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -240,7 +240,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="683857720"/>
+        <c:axId val="546427464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -276,7 +276,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="683921992"/>
+        <c:crossAx val="546434280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1376,7 +1376,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>